<commit_message>
Change Sqlite -> QtSQL approach. Remake create new macro function
</commit_message>
<xml_diff>
--- a/local_test/PasteTo.xlsx
+++ b/local_test/PasteTo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gtyohan/PycharmProjects/Auto_Financial_Reporting_1/local_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912312C3-D7F7-0843-855B-922A7689A566}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7996074C-228C-3D46-8480-0965BCC9A351}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10640" yWindow="7400" windowWidth="10000" windowHeight="6460" xr2:uid="{117BE157-6AE6-3146-9206-249AC8C4A531}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>